<commit_message>
Ajout des connecteurs de remplacement
</commit_message>
<xml_diff>
--- a/EL - Electrical/Autre/Faisceau/Cablage Optimus.xlsx
+++ b/EL - Electrical/Autre/Faisceau/Cablage Optimus.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EPSA\STUF2019\EL - Electrical\Autre\Faisceau\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C941960-0324-45BB-8CCB-3DD753E80225}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09E994D0-B063-4CA8-BE8E-9B6F7E664AB0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="238">
   <si>
     <t xml:space="preserve">Identification des câbles </t>
   </si>
@@ -716,6 +716,39 @@
   </si>
   <si>
     <t xml:space="preserve">Palette </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remplacé par </t>
+  </si>
+  <si>
+    <t>8STA71828S</t>
+  </si>
+  <si>
+    <t>8STA71828P</t>
+  </si>
+  <si>
+    <t>8STA01002S</t>
+  </si>
+  <si>
+    <t>8STA01002P</t>
+  </si>
+  <si>
+    <t>8STA70835S</t>
+  </si>
+  <si>
+    <t>8STA70835P</t>
+  </si>
+  <si>
+    <t>8STA61002P</t>
+  </si>
+  <si>
+    <t>8STA61002S</t>
+  </si>
+  <si>
+    <t>8STA01035P</t>
+  </si>
+  <si>
+    <t>8STA61035S</t>
   </si>
 </sst>
 </file>
@@ -777,7 +810,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -862,8 +895,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="24">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -1142,12 +1187,92 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1284,9 +1409,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1299,16 +1436,25 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1317,38 +1463,53 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1668,8 +1829,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Tableau7" displayName="Tableau7" ref="I21:K23" totalsRowShown="0">
-  <autoFilter ref="I21:K23" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Tableau7" displayName="Tableau7" ref="I23:K25" totalsRowShown="0">
+  <autoFilter ref="I23:K25" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Signal"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Quantité"/>
@@ -2579,8 +2740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21:G27"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2588,7 +2749,8 @@
     <col min="1" max="1" width="16.42578125" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" customWidth="1"/>
     <col min="3" max="3" width="13.140625" customWidth="1"/>
-    <col min="4" max="5" width="11.42578125"/>
+    <col min="4" max="4" width="11.42578125"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.85546875" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
     <col min="8" max="8" width="11.42578125"/>
@@ -2601,26 +2763,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="73" t="s">
         <v>222</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="E1" s="73" t="s">
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="E1" s="77" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="I1" s="74" t="s">
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="I1" s="78" t="s">
         <v>49</v>
       </c>
-      <c r="J1" s="74"/>
-      <c r="K1" s="74"/>
-      <c r="M1" s="75" t="s">
+      <c r="J1" s="78"/>
+      <c r="K1" s="78"/>
+      <c r="M1" s="79" t="s">
         <v>50</v>
       </c>
-      <c r="N1" s="75"/>
-      <c r="O1" s="75"/>
+      <c r="N1" s="79"/>
+      <c r="O1" s="79"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
@@ -2820,7 +2982,7 @@
       <c r="C7" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="76" t="s">
+      <c r="E7" s="80" t="s">
         <v>69</v>
       </c>
       <c r="F7" s="22" t="s">
@@ -2855,7 +3017,7 @@
       <c r="C8" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="76"/>
+      <c r="E8" s="80"/>
       <c r="F8" s="22" t="s">
         <v>72</v>
       </c>
@@ -2915,11 +3077,11 @@
       <c r="C10" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="79" t="s">
+      <c r="E10" s="75" t="s">
         <v>76</v>
       </c>
-      <c r="F10" s="79"/>
-      <c r="G10" s="79"/>
+      <c r="F10" s="75"/>
+      <c r="G10" s="75"/>
       <c r="I10" s="13" t="s">
         <v>77</v>
       </c>
@@ -2929,7 +3091,7 @@
       <c r="K10" t="s">
         <v>22</v>
       </c>
-      <c r="M10" s="80" t="s">
+      <c r="M10" s="76" t="s">
         <v>69</v>
       </c>
       <c r="N10" s="22" t="s">
@@ -2964,7 +3126,7 @@
       <c r="K11" t="s">
         <v>22</v>
       </c>
-      <c r="M11" s="80"/>
+      <c r="M11" s="76"/>
       <c r="N11" s="22" t="s">
         <v>81</v>
       </c>
@@ -3021,7 +3183,7 @@
       </c>
     </row>
     <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="80" t="s">
+      <c r="A14" s="76" t="s">
         <v>69</v>
       </c>
       <c r="B14" s="24" t="s">
@@ -3041,9 +3203,9 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="80"/>
-      <c r="B15" s="24" t="s">
+    <row r="15" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="99"/>
+      <c r="B15" s="98" t="s">
         <v>221</v>
       </c>
       <c r="E15" t="s">
@@ -3056,7 +3218,13 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="100" t="s">
+        <v>227</v>
+      </c>
+      <c r="B16" s="97" t="s">
+        <v>228</v>
+      </c>
       <c r="E16" t="s">
         <v>85</v>
       </c>
@@ -3076,7 +3244,11 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="101"/>
+      <c r="B17" s="96" t="s">
+        <v>229</v>
+      </c>
       <c r="E17" s="31" t="s">
         <v>66</v>
       </c>
@@ -3084,96 +3256,109 @@
         <f>SUM(F12:F16)</f>
         <v>9</v>
       </c>
-      <c r="I17" s="80" t="s">
+      <c r="I17" s="76" t="s">
         <v>69</v>
       </c>
       <c r="J17" s="22" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E18" s="80" t="s">
+    <row r="18" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="95"/>
+      <c r="B18" s="95"/>
+      <c r="E18" s="76" t="s">
         <v>69</v>
       </c>
       <c r="F18" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="I18" s="80"/>
+      <c r="I18" s="76"/>
       <c r="J18" s="22" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C19" s="13"/>
-      <c r="E19" s="80"/>
+      <c r="E19" s="76"/>
       <c r="F19" s="22" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="I20" s="77" t="s">
+      <c r="H19" s="102"/>
+      <c r="I19" s="100" t="s">
+        <v>227</v>
+      </c>
+      <c r="J19" s="110" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D20" s="108"/>
+      <c r="E20" s="100" t="s">
+        <v>227</v>
+      </c>
+      <c r="F20" s="103" t="s">
+        <v>231</v>
+      </c>
+      <c r="G20" s="104"/>
+      <c r="H20" s="102"/>
+      <c r="I20" s="101"/>
+      <c r="J20" s="111" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="E21" s="109"/>
+      <c r="F21" s="105" t="s">
+        <v>235</v>
+      </c>
+      <c r="G21" s="23"/>
+    </row>
+    <row r="22" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E22" s="109"/>
+      <c r="F22" s="22" t="s">
+        <v>236</v>
+      </c>
+      <c r="G22" s="106"/>
+      <c r="I22" s="72" t="s">
         <v>96</v>
       </c>
-      <c r="J20" s="77"/>
-      <c r="K20" s="77"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="23"/>
-      <c r="I21" s="13" t="s">
+      <c r="J22" s="72"/>
+      <c r="K22" s="72"/>
+    </row>
+    <row r="23" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D23" s="108"/>
+      <c r="E23" s="101"/>
+      <c r="F23" s="22" t="s">
+        <v>237</v>
+      </c>
+      <c r="G23" s="106"/>
+      <c r="I23" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="J21" s="13" t="s">
+      <c r="J23" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="K21" s="13" t="s">
+      <c r="K23" s="13" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E22" s="23"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="23"/>
-      <c r="I22" s="33" t="s">
+    <row r="24" spans="1:11" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="73" t="s">
+        <v>99</v>
+      </c>
+      <c r="B24" s="73"/>
+      <c r="C24" s="73"/>
+      <c r="E24" s="107"/>
+      <c r="F24" s="107"/>
+      <c r="G24" s="23"/>
+      <c r="I24" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="J22">
+      <c r="J24">
         <v>1</v>
       </c>
-      <c r="K22" t="s">
+      <c r="K24" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E23" s="23"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="23"/>
-      <c r="I23" t="s">
-        <v>98</v>
-      </c>
-      <c r="J23">
-        <v>2</v>
-      </c>
-      <c r="K23" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A24" s="72" t="s">
-        <v>99</v>
-      </c>
-      <c r="B24" s="72"/>
-      <c r="C24" s="72"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="23"/>
-      <c r="G24" s="23"/>
-      <c r="I24" s="34" t="s">
-        <v>66</v>
-      </c>
-      <c r="J24" s="21">
-        <f>SUM(J22:J23)</f>
-        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -3189,14 +3374,17 @@
       <c r="E25" s="23"/>
       <c r="F25" s="23"/>
       <c r="G25" s="23"/>
-      <c r="I25" s="27" t="s">
-        <v>69</v>
-      </c>
-      <c r="J25" s="22" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I25" t="s">
+        <v>98</v>
+      </c>
+      <c r="J25">
+        <v>2</v>
+      </c>
+      <c r="K25" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
         <v>101</v>
       </c>
@@ -3209,9 +3397,12 @@
       <c r="E26" s="23"/>
       <c r="F26" s="23"/>
       <c r="G26" s="23"/>
-      <c r="I26" s="27"/>
-      <c r="J26" s="22" t="s">
-        <v>102</v>
+      <c r="I26" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="J26" s="21">
+        <f>SUM(J24:J25)</f>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -3224,6 +3415,12 @@
       <c r="C27" s="36" t="s">
         <v>22</v>
       </c>
+      <c r="I27" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="J27" s="22" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="23" t="s">
@@ -3235,6 +3432,10 @@
       <c r="C28" s="36" t="s">
         <v>22</v>
       </c>
+      <c r="I28" s="27"/>
+      <c r="J28" s="22" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="29" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
@@ -3247,25 +3448,39 @@
       <c r="C29" s="37"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="94" t="s">
         <v>69</v>
       </c>
       <c r="B30" s="22" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="27"/>
+    <row r="31" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="94"/>
       <c r="B31" s="22" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="78" t="s">
+    <row r="32" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="100" t="s">
+        <v>227</v>
+      </c>
+      <c r="B32" s="110" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="101"/>
+      <c r="B33" s="111" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="74" t="s">
         <v>105</v>
       </c>
-      <c r="B34" s="78"/>
-      <c r="C34" s="78"/>
+      <c r="B34" s="74"/>
+      <c r="C34" s="74"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
@@ -3371,8 +3586,13 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="I20:K20"/>
+  <mergeCells count="18">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="I22:K22"/>
     <mergeCell ref="A24:C24"/>
     <mergeCell ref="A34:C34"/>
     <mergeCell ref="E10:G10"/>
@@ -3380,11 +3600,11 @@
     <mergeCell ref="I17:I18"/>
     <mergeCell ref="E18:E19"/>
     <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="E20:E23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3405,7 +3625,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18:F19"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3439,220 +3659,220 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="85"/>
+      <c r="A2" s="81"/>
       <c r="B2" s="61" t="s">
         <v>224</v>
       </c>
       <c r="C2" s="44"/>
       <c r="D2" s="44"/>
-      <c r="E2" s="90" t="s">
+      <c r="E2" s="87" t="s">
         <v>223</v>
       </c>
-      <c r="F2" s="81">
+      <c r="F2" s="88">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="85"/>
+      <c r="A3" s="81"/>
       <c r="B3" s="62" t="s">
         <v>225</v>
       </c>
       <c r="C3" s="45"/>
       <c r="D3" s="45"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="81"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="88"/>
     </row>
     <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="85"/>
+      <c r="A4" s="81"/>
       <c r="B4" s="63" t="s">
         <v>214</v>
       </c>
       <c r="C4" s="46"/>
       <c r="D4" s="46"/>
-      <c r="E4" s="82" t="s">
+      <c r="E4" s="89" t="s">
         <v>120</v>
       </c>
-      <c r="F4" s="81">
+      <c r="F4" s="88">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="85"/>
+      <c r="A5" s="81"/>
       <c r="B5" s="64" t="s">
         <v>215</v>
       </c>
       <c r="C5" s="47"/>
       <c r="D5" s="47"/>
-      <c r="E5" s="82"/>
-      <c r="F5" s="81"/>
+      <c r="E5" s="89"/>
+      <c r="F5" s="88"/>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="85"/>
+      <c r="A6" s="81"/>
       <c r="B6" s="65" t="s">
         <v>122</v>
       </c>
       <c r="C6" s="48"/>
       <c r="D6" s="48"/>
-      <c r="E6" s="91" t="s">
+      <c r="E6" s="90" t="s">
         <v>123</v>
       </c>
-      <c r="F6" s="81">
+      <c r="F6" s="88">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="85"/>
+      <c r="A7" s="81"/>
       <c r="B7" s="65" t="s">
         <v>124</v>
       </c>
       <c r="C7" s="48"/>
       <c r="D7" s="48"/>
-      <c r="E7" s="91"/>
-      <c r="F7" s="81"/>
+      <c r="E7" s="90"/>
+      <c r="F7" s="88"/>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="85"/>
+      <c r="A8" s="81"/>
       <c r="B8" s="40" t="s">
         <v>125</v>
       </c>
       <c r="C8" s="41"/>
       <c r="D8" s="41"/>
-      <c r="E8" s="92" t="s">
+      <c r="E8" s="91" t="s">
         <v>48</v>
       </c>
-      <c r="F8" s="81">
+      <c r="F8" s="88">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="85"/>
+      <c r="A9" s="81"/>
       <c r="B9" s="42" t="s">
         <v>126</v>
       </c>
       <c r="C9" s="43"/>
       <c r="D9" s="43"/>
-      <c r="E9" s="92"/>
-      <c r="F9" s="81"/>
+      <c r="E9" s="91"/>
+      <c r="F9" s="88"/>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="85"/>
+      <c r="A10" s="81"/>
       <c r="B10" s="61" t="s">
         <v>127</v>
       </c>
       <c r="C10" s="44"/>
       <c r="D10" s="44"/>
-      <c r="E10" s="90" t="s">
+      <c r="E10" s="87" t="s">
         <v>128</v>
       </c>
-      <c r="F10" s="81">
+      <c r="F10" s="88">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="85"/>
+      <c r="A11" s="81"/>
       <c r="B11" s="62" t="s">
         <v>119</v>
       </c>
       <c r="C11" s="45"/>
       <c r="D11" s="45"/>
-      <c r="E11" s="90"/>
-      <c r="F11" s="81"/>
+      <c r="E11" s="87"/>
+      <c r="F11" s="88"/>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="85"/>
+      <c r="A12" s="81"/>
       <c r="B12" s="49" t="s">
         <v>129</v>
       </c>
       <c r="C12" s="50"/>
       <c r="D12" s="50"/>
-      <c r="E12" s="93" t="s">
+      <c r="E12" s="92" t="s">
         <v>130</v>
       </c>
-      <c r="F12" s="81">
+      <c r="F12" s="88">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="85"/>
+      <c r="A13" s="81"/>
       <c r="B13" s="49" t="s">
         <v>131</v>
       </c>
       <c r="C13" s="50"/>
       <c r="D13" s="50"/>
-      <c r="E13" s="93"/>
-      <c r="F13" s="81"/>
+      <c r="E13" s="92"/>
+      <c r="F13" s="88"/>
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="85"/>
+      <c r="A14" s="81"/>
       <c r="B14" s="63" t="s">
         <v>132</v>
       </c>
       <c r="C14" s="46"/>
       <c r="D14" s="46"/>
-      <c r="E14" s="82" t="s">
+      <c r="E14" s="89" t="s">
         <v>133</v>
       </c>
-      <c r="F14" s="81">
+      <c r="F14" s="88">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="85"/>
+      <c r="A15" s="81"/>
       <c r="B15" s="64" t="s">
         <v>121</v>
       </c>
       <c r="C15" s="47"/>
       <c r="D15" s="47"/>
-      <c r="E15" s="82"/>
-      <c r="F15" s="81"/>
+      <c r="E15" s="89"/>
+      <c r="F15" s="88"/>
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="85"/>
+      <c r="A16" s="81"/>
       <c r="B16" s="40" t="s">
         <v>134</v>
       </c>
       <c r="C16" s="41"/>
       <c r="D16" s="41"/>
-      <c r="E16" s="83" t="s">
+      <c r="E16" s="93" t="s">
         <v>50</v>
       </c>
-      <c r="F16" s="84">
+      <c r="F16" s="83">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="85"/>
+      <c r="A17" s="81"/>
       <c r="B17" s="66" t="s">
         <v>135</v>
       </c>
       <c r="C17" s="50"/>
       <c r="D17" s="50"/>
-      <c r="E17" s="83"/>
-      <c r="F17" s="84"/>
+      <c r="E17" s="93"/>
+      <c r="F17" s="83"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="85"/>
+      <c r="A18" s="81"/>
       <c r="B18" s="67" t="s">
         <v>218</v>
       </c>
       <c r="C18" s="58"/>
       <c r="D18" s="58"/>
-      <c r="E18" s="88" t="s">
+      <c r="E18" s="85" t="s">
         <v>219</v>
       </c>
-      <c r="F18" s="84">
+      <c r="F18" s="83">
         <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="86"/>
+      <c r="A19" s="82"/>
       <c r="B19" s="68" t="s">
         <v>217</v>
       </c>
       <c r="C19" s="59"/>
       <c r="D19" s="59"/>
-      <c r="E19" s="89"/>
-      <c r="F19" s="87"/>
+      <c r="E19" s="86"/>
+      <c r="F19" s="84"/>
     </row>
     <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E20" s="57" t="s">
@@ -3665,6 +3885,9 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="F16:F17"/>
     <mergeCell ref="A2:A19"/>
     <mergeCell ref="F18:F19"/>
     <mergeCell ref="E18:E19"/>
@@ -3681,9 +3904,6 @@
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="F12:F13"/>
     <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="F16:F17"/>
   </mergeCells>
   <conditionalFormatting sqref="C10:C18 D10:D20 C2:D9">
     <cfRule type="containsText" dxfId="16" priority="2" operator="containsText" text="'Oui'"/>

</xml_diff>

<commit_message>
modif signaux connecteurs pare-feu
</commit_message>
<xml_diff>
--- a/EL - Electrical/Autre/Faisceau/Cablage Optimus.xlsx
+++ b/EL - Electrical/Autre/Faisceau/Cablage Optimus.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EPSA\STUF2019\EL - Electrical\Autre\Faisceau\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09E994D0-B063-4CA8-BE8E-9B6F7E664AB0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24B402C6-0D42-4E82-9845-C298CC7F9E84}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cablage" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="239">
   <si>
     <t xml:space="preserve">Identification des câbles </t>
   </si>
@@ -749,6 +749,9 @@
   </si>
   <si>
     <t>8STA61035S</t>
+  </si>
+  <si>
+    <t>Front brake pressure</t>
   </si>
 </sst>
 </file>
@@ -1272,7 +1275,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1409,88 +1412,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1502,14 +1426,92 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1769,8 +1771,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="A2:C12" totalsRowShown="0">
-  <autoFilter ref="A2:C12" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="A2:C13" totalsRowShown="0">
+  <autoFilter ref="A2:C13" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Signal"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Quantité"/>
@@ -2740,8 +2742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="A16:XFD16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2763,26 +2765,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="84" t="s">
         <v>222</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="E1" s="77" t="s">
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="E1" s="85" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="I1" s="78" t="s">
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="I1" s="86" t="s">
         <v>49</v>
       </c>
-      <c r="J1" s="78"/>
-      <c r="K1" s="78"/>
-      <c r="M1" s="79" t="s">
+      <c r="J1" s="86"/>
+      <c r="K1" s="86"/>
+      <c r="M1" s="87" t="s">
         <v>50</v>
       </c>
-      <c r="N1" s="79"/>
-      <c r="O1" s="79"/>
+      <c r="N1" s="87"/>
+      <c r="O1" s="87"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
@@ -2982,7 +2984,7 @@
       <c r="C7" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="80" t="s">
+      <c r="E7" s="88" t="s">
         <v>69</v>
       </c>
       <c r="F7" s="22" t="s">
@@ -3017,7 +3019,7 @@
       <c r="C8" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="80"/>
+      <c r="E8" s="88"/>
       <c r="F8" s="22" t="s">
         <v>72</v>
       </c>
@@ -3077,11 +3079,11 @@
       <c r="C10" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="75" t="s">
+      <c r="E10" s="91" t="s">
         <v>76</v>
       </c>
-      <c r="F10" s="75"/>
-      <c r="G10" s="75"/>
+      <c r="F10" s="91"/>
+      <c r="G10" s="91"/>
       <c r="I10" s="13" t="s">
         <v>77</v>
       </c>
@@ -3091,7 +3093,7 @@
       <c r="K10" t="s">
         <v>22</v>
       </c>
-      <c r="M10" s="76" t="s">
+      <c r="M10" s="92" t="s">
         <v>69</v>
       </c>
       <c r="N10" s="22" t="s">
@@ -3126,7 +3128,7 @@
       <c r="K11" t="s">
         <v>22</v>
       </c>
-      <c r="M11" s="76"/>
+      <c r="M11" s="92"/>
       <c r="N11" s="22" t="s">
         <v>81</v>
       </c>
@@ -3159,12 +3161,14 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="B13" s="32">
-        <f>SUM(Tableau1[Quantité])</f>
-        <v>17</v>
+      <c r="A13" t="s">
+        <v>238</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>22</v>
       </c>
       <c r="E13" t="s">
         <v>84</v>
@@ -3183,11 +3187,12 @@
       </c>
     </row>
     <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="76" t="s">
-        <v>69</v>
-      </c>
-      <c r="B14" s="24" t="s">
-        <v>220</v>
+      <c r="A14" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" s="32">
+        <f>SUM(Tableau1[Quantité])</f>
+        <v>18</v>
       </c>
       <c r="E14" t="s">
         <v>57</v>
@@ -3203,10 +3208,12 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="99"/>
-      <c r="B15" s="98" t="s">
-        <v>221</v>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="92" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="24" t="s">
+        <v>220</v>
       </c>
       <c r="E15" t="s">
         <v>87</v>
@@ -3218,12 +3225,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="100" t="s">
-        <v>227</v>
-      </c>
-      <c r="B16" s="97" t="s">
-        <v>228</v>
+    <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="93"/>
+      <c r="B16" s="74" t="s">
+        <v>221</v>
       </c>
       <c r="E16" t="s">
         <v>85</v>
@@ -3244,10 +3249,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="101"/>
-      <c r="B17" s="96" t="s">
-        <v>229</v>
+    <row r="17" spans="1:11" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="94" t="s">
+        <v>227</v>
+      </c>
+      <c r="B17" s="73" t="s">
+        <v>228</v>
       </c>
       <c r="E17" s="31" t="s">
         <v>66</v>
@@ -3256,82 +3263,84 @@
         <f>SUM(F12:F16)</f>
         <v>9</v>
       </c>
-      <c r="I17" s="76" t="s">
+      <c r="I17" s="92" t="s">
         <v>69</v>
       </c>
       <c r="J17" s="22" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="95"/>
-      <c r="B18" s="95"/>
-      <c r="E18" s="76" t="s">
+      <c r="B18" s="72" t="s">
+        <v>229</v>
+      </c>
+      <c r="E18" s="92" t="s">
         <v>69</v>
       </c>
       <c r="F18" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="I18" s="76"/>
+      <c r="I18" s="92"/>
       <c r="J18" s="22" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C19" s="13"/>
-      <c r="E19" s="76"/>
+      <c r="E19" s="92"/>
       <c r="F19" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="H19" s="102"/>
-      <c r="I19" s="100" t="s">
+      <c r="H19" s="75"/>
+      <c r="I19" s="94" t="s">
         <v>227</v>
       </c>
-      <c r="J19" s="110" t="s">
+      <c r="J19" s="82" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D20" s="108"/>
-      <c r="E20" s="100" t="s">
+      <c r="D20" s="81"/>
+      <c r="E20" s="94" t="s">
         <v>227</v>
       </c>
-      <c r="F20" s="103" t="s">
+      <c r="F20" s="76" t="s">
         <v>231</v>
       </c>
-      <c r="G20" s="104"/>
-      <c r="H20" s="102"/>
-      <c r="I20" s="101"/>
-      <c r="J20" s="111" t="s">
+      <c r="G20" s="77"/>
+      <c r="H20" s="75"/>
+      <c r="I20" s="95"/>
+      <c r="J20" s="83" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="E21" s="109"/>
-      <c r="F21" s="105" t="s">
+      <c r="E21" s="97"/>
+      <c r="F21" s="78" t="s">
         <v>235</v>
       </c>
       <c r="G21" s="23"/>
     </row>
     <row r="22" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E22" s="109"/>
+      <c r="E22" s="97"/>
       <c r="F22" s="22" t="s">
         <v>236</v>
       </c>
-      <c r="G22" s="106"/>
-      <c r="I22" s="72" t="s">
+      <c r="G22" s="79"/>
+      <c r="I22" s="89" t="s">
         <v>96</v>
       </c>
-      <c r="J22" s="72"/>
-      <c r="K22" s="72"/>
+      <c r="J22" s="89"/>
+      <c r="K22" s="89"/>
     </row>
     <row r="23" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D23" s="108"/>
-      <c r="E23" s="101"/>
+      <c r="D23" s="81"/>
+      <c r="E23" s="95"/>
       <c r="F23" s="22" t="s">
         <v>237</v>
       </c>
-      <c r="G23" s="106"/>
+      <c r="G23" s="79"/>
       <c r="I23" s="13" t="s">
         <v>51</v>
       </c>
@@ -3343,13 +3352,13 @@
       </c>
     </row>
     <row r="24" spans="1:11" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="73" t="s">
+      <c r="A24" s="84" t="s">
         <v>99</v>
       </c>
-      <c r="B24" s="73"/>
-      <c r="C24" s="73"/>
-      <c r="E24" s="107"/>
-      <c r="F24" s="107"/>
+      <c r="B24" s="84"/>
+      <c r="C24" s="84"/>
+      <c r="E24" s="80"/>
+      <c r="F24" s="80"/>
       <c r="G24" s="23"/>
       <c r="I24" s="33" t="s">
         <v>97</v>
@@ -3448,7 +3457,7 @@
       <c r="C29" s="37"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="94" t="s">
+      <c r="A30" s="96" t="s">
         <v>69</v>
       </c>
       <c r="B30" s="22" t="s">
@@ -3456,31 +3465,31 @@
       </c>
     </row>
     <row r="31" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="94"/>
+      <c r="A31" s="96"/>
       <c r="B31" s="22" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="100" t="s">
+      <c r="A32" s="94" t="s">
         <v>227</v>
       </c>
-      <c r="B32" s="110" t="s">
+      <c r="B32" s="82" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="101"/>
-      <c r="B33" s="111" t="s">
+      <c r="A33" s="95"/>
+      <c r="B33" s="83" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="74" t="s">
+      <c r="A34" s="90" t="s">
         <v>105</v>
       </c>
-      <c r="B34" s="74"/>
-      <c r="C34" s="74"/>
+      <c r="B34" s="90"/>
+      <c r="C34" s="90"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
@@ -3587,11 +3596,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="E7:E8"/>
     <mergeCell ref="I22:K22"/>
     <mergeCell ref="A24:C24"/>
     <mergeCell ref="A34:C34"/>
@@ -3599,12 +3603,17 @@
     <mergeCell ref="M10:M11"/>
     <mergeCell ref="I17:I18"/>
     <mergeCell ref="E18:E19"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A16:A17"/>
     <mergeCell ref="I19:I20"/>
     <mergeCell ref="A30:A31"/>
     <mergeCell ref="A32:A33"/>
     <mergeCell ref="E20:E23"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="E7:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3659,220 +3668,220 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="81"/>
+      <c r="A2" s="101"/>
       <c r="B2" s="61" t="s">
         <v>224</v>
       </c>
       <c r="C2" s="44"/>
       <c r="D2" s="44"/>
-      <c r="E2" s="87" t="s">
+      <c r="E2" s="106" t="s">
         <v>223</v>
       </c>
-      <c r="F2" s="88">
+      <c r="F2" s="98">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="81"/>
+      <c r="A3" s="101"/>
       <c r="B3" s="62" t="s">
         <v>225</v>
       </c>
       <c r="C3" s="45"/>
       <c r="D3" s="45"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="88"/>
+      <c r="E3" s="106"/>
+      <c r="F3" s="98"/>
     </row>
     <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="81"/>
+      <c r="A4" s="101"/>
       <c r="B4" s="63" t="s">
         <v>214</v>
       </c>
       <c r="C4" s="46"/>
       <c r="D4" s="46"/>
-      <c r="E4" s="89" t="s">
+      <c r="E4" s="107" t="s">
         <v>120</v>
       </c>
-      <c r="F4" s="88">
+      <c r="F4" s="98">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="81"/>
+      <c r="A5" s="101"/>
       <c r="B5" s="64" t="s">
         <v>215</v>
       </c>
       <c r="C5" s="47"/>
       <c r="D5" s="47"/>
-      <c r="E5" s="89"/>
-      <c r="F5" s="88"/>
+      <c r="E5" s="107"/>
+      <c r="F5" s="98"/>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="81"/>
+      <c r="A6" s="101"/>
       <c r="B6" s="65" t="s">
         <v>122</v>
       </c>
       <c r="C6" s="48"/>
       <c r="D6" s="48"/>
-      <c r="E6" s="90" t="s">
+      <c r="E6" s="108" t="s">
         <v>123</v>
       </c>
-      <c r="F6" s="88">
+      <c r="F6" s="98">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="81"/>
+      <c r="A7" s="101"/>
       <c r="B7" s="65" t="s">
         <v>124</v>
       </c>
       <c r="C7" s="48"/>
       <c r="D7" s="48"/>
-      <c r="E7" s="90"/>
-      <c r="F7" s="88"/>
+      <c r="E7" s="108"/>
+      <c r="F7" s="98"/>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="81"/>
+      <c r="A8" s="101"/>
       <c r="B8" s="40" t="s">
         <v>125</v>
       </c>
       <c r="C8" s="41"/>
       <c r="D8" s="41"/>
-      <c r="E8" s="91" t="s">
+      <c r="E8" s="109" t="s">
         <v>48</v>
       </c>
-      <c r="F8" s="88">
+      <c r="F8" s="98">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="81"/>
+      <c r="A9" s="101"/>
       <c r="B9" s="42" t="s">
         <v>126</v>
       </c>
       <c r="C9" s="43"/>
       <c r="D9" s="43"/>
-      <c r="E9" s="91"/>
-      <c r="F9" s="88"/>
+      <c r="E9" s="109"/>
+      <c r="F9" s="98"/>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="81"/>
+      <c r="A10" s="101"/>
       <c r="B10" s="61" t="s">
         <v>127</v>
       </c>
       <c r="C10" s="44"/>
       <c r="D10" s="44"/>
-      <c r="E10" s="87" t="s">
+      <c r="E10" s="106" t="s">
         <v>128</v>
       </c>
-      <c r="F10" s="88">
+      <c r="F10" s="98">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="81"/>
+      <c r="A11" s="101"/>
       <c r="B11" s="62" t="s">
         <v>119</v>
       </c>
       <c r="C11" s="45"/>
       <c r="D11" s="45"/>
-      <c r="E11" s="87"/>
-      <c r="F11" s="88"/>
+      <c r="E11" s="106"/>
+      <c r="F11" s="98"/>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="81"/>
+      <c r="A12" s="101"/>
       <c r="B12" s="49" t="s">
         <v>129</v>
       </c>
       <c r="C12" s="50"/>
       <c r="D12" s="50"/>
-      <c r="E12" s="92" t="s">
+      <c r="E12" s="110" t="s">
         <v>130</v>
       </c>
-      <c r="F12" s="88">
+      <c r="F12" s="98">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="81"/>
+      <c r="A13" s="101"/>
       <c r="B13" s="49" t="s">
         <v>131</v>
       </c>
       <c r="C13" s="50"/>
       <c r="D13" s="50"/>
-      <c r="E13" s="92"/>
-      <c r="F13" s="88"/>
+      <c r="E13" s="110"/>
+      <c r="F13" s="98"/>
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="81"/>
+      <c r="A14" s="101"/>
       <c r="B14" s="63" t="s">
         <v>132</v>
       </c>
       <c r="C14" s="46"/>
       <c r="D14" s="46"/>
-      <c r="E14" s="89" t="s">
+      <c r="E14" s="107" t="s">
         <v>133</v>
       </c>
-      <c r="F14" s="88">
+      <c r="F14" s="98">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="81"/>
+      <c r="A15" s="101"/>
       <c r="B15" s="64" t="s">
         <v>121</v>
       </c>
       <c r="C15" s="47"/>
       <c r="D15" s="47"/>
-      <c r="E15" s="89"/>
-      <c r="F15" s="88"/>
+      <c r="E15" s="107"/>
+      <c r="F15" s="98"/>
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="81"/>
+      <c r="A16" s="101"/>
       <c r="B16" s="40" t="s">
         <v>134</v>
       </c>
       <c r="C16" s="41"/>
       <c r="D16" s="41"/>
-      <c r="E16" s="93" t="s">
+      <c r="E16" s="99" t="s">
         <v>50</v>
       </c>
-      <c r="F16" s="83">
+      <c r="F16" s="100">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="81"/>
+      <c r="A17" s="101"/>
       <c r="B17" s="66" t="s">
         <v>135</v>
       </c>
       <c r="C17" s="50"/>
       <c r="D17" s="50"/>
-      <c r="E17" s="93"/>
-      <c r="F17" s="83"/>
+      <c r="E17" s="99"/>
+      <c r="F17" s="100"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="81"/>
+      <c r="A18" s="101"/>
       <c r="B18" s="67" t="s">
         <v>218</v>
       </c>
       <c r="C18" s="58"/>
       <c r="D18" s="58"/>
-      <c r="E18" s="85" t="s">
+      <c r="E18" s="104" t="s">
         <v>219</v>
       </c>
-      <c r="F18" s="83">
+      <c r="F18" s="100">
         <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="82"/>
+      <c r="A19" s="102"/>
       <c r="B19" s="68" t="s">
         <v>217</v>
       </c>
       <c r="C19" s="59"/>
       <c r="D19" s="59"/>
-      <c r="E19" s="86"/>
-      <c r="F19" s="84"/>
+      <c r="E19" s="105"/>
+      <c r="F19" s="103"/>
     </row>
     <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E20" s="57" t="s">
@@ -3885,6 +3894,9 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="E14:E15"/>
     <mergeCell ref="F14:F15"/>
     <mergeCell ref="E16:E17"/>
     <mergeCell ref="F16:F17"/>
@@ -3901,9 +3913,6 @@
     <mergeCell ref="F8:F9"/>
     <mergeCell ref="E10:E11"/>
     <mergeCell ref="F10:F11"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="E14:E15"/>
   </mergeCells>
   <conditionalFormatting sqref="C10:C18 D10:D20 C2:D9">
     <cfRule type="containsText" dxfId="16" priority="2" operator="containsText" text="'Oui'"/>

</xml_diff>